<commit_message>
First version that generates some output from club records as input
</commit_message>
<xml_diff>
--- a/prev_known_and_20022_club_records.xlsx
+++ b/prev_known_and_20022_club_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5460C231-6AB4-4416-BD7E-EEEA2D98DD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC946F56-938A-4913-BB86-A69DA59047D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="175">
   <si>
     <r>
       <t>C&amp;C AC Track and Field records  - Overall club records</t>
@@ -491,6 +491,153 @@
   </si>
   <si>
     <t xml:space="preserve">https://more.arrs.run/runner/15799 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.43 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.70 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">47.14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:46.18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:35.93 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:36.08 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:05.13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27:10.41 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:59.86 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.92 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">51.37 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:54.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:35.8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.05 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.52 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.56 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">50.95 </t>
+  </si>
+  <si>
+    <t>69.78</t>
+  </si>
+  <si>
+    <t>58.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62.54 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">43.6 </t>
+  </si>
+  <si>
+    <t>4974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:27.0 </t>
+  </si>
+  <si>
+    <t>2582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53.91 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:03.94 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:07.20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:19.8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:45.87 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">32:25.34 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:36.7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">59.7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:26.9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:58.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.72  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.75 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.55 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.99 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.16 </t>
+  </si>
+  <si>
+    <t>44.30</t>
+  </si>
+  <si>
+    <t>39.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3051 pts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">44.48 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.61 </t>
+  </si>
+  <si>
+    <t>3:59.1</t>
+  </si>
+  <si>
+    <t>Use text format when pasting numbers from club records sheet!</t>
   </si>
 </sst>
 </file>
@@ -631,7 +778,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -645,51 +792,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="47" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1005,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0672E4C-1F81-4344-8F80-ED5988EB27BD}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1035,13 +1176,13 @@
       <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1052,19 +1193,19 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6">
-        <v>10.43</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="D2" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="9">
         <v>2022</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="10">
         <v>100</v>
       </c>
       <c r="H2" t="s">
@@ -1075,19 +1216,19 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6">
-        <v>20.7</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="D3" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="9">
         <v>1990</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="10">
         <v>200</v>
       </c>
       <c r="H3" t="s">
@@ -1098,19 +1239,22 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6">
-        <v>47.14</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="9">
         <v>1989</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="10">
         <v>400</v>
       </c>
       <c r="H4" t="s">
@@ -1121,19 +1265,19 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7">
-        <v>1.2289351851851851E-3</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="9">
         <v>2022</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="10">
         <v>800</v>
       </c>
       <c r="H5" t="s">
@@ -1144,19 +1288,19 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7">
-        <v>2.4991898148148148E-3</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="D6" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="9">
         <v>2020</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="10">
         <v>1500</v>
       </c>
       <c r="H6" t="s">
@@ -1167,19 +1311,19 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="7">
-        <v>5.278703703703703E-3</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D7" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="9">
         <v>2021</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="10">
         <v>3000</v>
       </c>
       <c r="H7" t="s">
@@ -1190,19 +1334,19 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7">
-        <v>9.0871527777777773E-3</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="D8" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="9">
         <v>2021</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="10">
         <v>5000</v>
       </c>
       <c r="H8" t="s">
@@ -1213,19 +1357,19 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="7">
-        <v>1.8870486111111112E-2</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D9" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="9">
         <v>2021</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="10">
         <v>10000</v>
       </c>
       <c r="H9" t="s">
@@ -1236,19 +1380,19 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="7">
-        <v>2.7761574074074073E-3</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="D10" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="9">
         <v>2021</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10" t="s">
         <v>87</v>
       </c>
       <c r="H10" t="s">
@@ -1259,19 +1403,19 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="6">
-        <v>13.92</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="D11" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="9">
         <v>1984</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="11" t="s">
         <v>88</v>
       </c>
       <c r="H11" t="s">
@@ -1282,19 +1426,19 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="6">
-        <v>13.92</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="D12" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="9">
         <v>2012</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="11" t="s">
         <v>88</v>
       </c>
       <c r="H12" t="s">
@@ -1305,19 +1449,19 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="6">
-        <v>51.37</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="D13" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="9">
         <v>2022</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="10" t="s">
         <v>89</v>
       </c>
       <c r="H13" t="s">
@@ -1328,19 +1472,19 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="7">
-        <v>4.0972222222222226E-3</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="D14" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="9">
         <v>1969</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="10" t="s">
         <v>90</v>
       </c>
       <c r="H14" t="s">
@@ -1351,19 +1495,19 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="7">
-        <v>5.9699074074074064E-3</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="D15" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="9">
         <v>1977</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="10" t="s">
         <v>91</v>
       </c>
       <c r="H15" t="s">
@@ -1374,19 +1518,19 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="6">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="D16" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="9">
         <v>1977</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="10" t="s">
         <v>92</v>
       </c>
       <c r="H16" t="s">
@@ -1397,19 +1541,19 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="6">
-        <v>7.12</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="9">
         <v>1968</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="10" t="s">
         <v>93</v>
       </c>
       <c r="H17" t="s">
@@ -1420,19 +1564,19 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="6">
-        <v>15.52</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D18" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="9">
         <v>1978</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="10" t="s">
         <v>94</v>
       </c>
       <c r="H18" t="s">
@@ -1443,19 +1587,19 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="6">
-        <v>4.2</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="9">
         <v>1982</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="10" t="s">
         <v>95</v>
       </c>
       <c r="H19" t="s">
@@ -1466,19 +1610,19 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="6">
-        <v>16.559999999999999</v>
-      </c>
-      <c r="E20" s="6">
+      <c r="D20" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" s="9">
         <v>1969</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="10" t="s">
         <v>96</v>
       </c>
       <c r="H20" t="s">
@@ -1489,19 +1633,19 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="6">
-        <v>50.95</v>
-      </c>
-      <c r="E21" s="6">
+      <c r="D21" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="9">
         <v>2022</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="10" t="s">
         <v>120</v>
       </c>
       <c r="H21" t="s">
@@ -1512,11 +1656,11 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="13">
-        <v>69.78</v>
+      <c r="D22" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="E22" s="13">
         <v>1971</v>
@@ -1524,7 +1668,7 @@
       <c r="F22" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="10" t="s">
         <v>111</v>
       </c>
       <c r="H22" t="s">
@@ -1535,19 +1679,19 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="5">
-        <v>58.44</v>
-      </c>
-      <c r="E23" s="5">
+      <c r="D23" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="8">
         <v>1990</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="10" t="s">
         <v>112</v>
       </c>
       <c r="H23" t="s">
@@ -1558,19 +1702,19 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="6">
-        <v>62.54</v>
-      </c>
-      <c r="E24" s="6">
+      <c r="D24" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="9">
         <v>1970</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="10" t="s">
         <v>113</v>
       </c>
       <c r="H24" t="s">
@@ -1581,19 +1725,19 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="6">
-        <v>2582</v>
-      </c>
-      <c r="E25" s="6">
+      <c r="D25" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25" s="9">
         <v>2008</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="10" t="s">
         <v>114</v>
       </c>
       <c r="H25" t="s">
@@ -1604,19 +1748,19 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="6">
-        <v>4974</v>
-      </c>
-      <c r="E26" s="6">
+      <c r="D26" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="9">
         <v>2022</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="11" t="s">
         <v>99</v>
       </c>
       <c r="H26" t="s">
@@ -1627,19 +1771,19 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="6">
-        <v>43.6</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="D27" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="11" t="s">
         <v>115</v>
       </c>
       <c r="H27" t="s">
@@ -1650,19 +1794,19 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="7">
-        <v>2.3958333333333336E-3</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="D28" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="11" t="s">
         <v>116</v>
       </c>
       <c r="H28" t="s">
@@ -1676,71 +1820,71 @@
       <c r="B29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="17">
         <v>2017</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="10">
         <v>100</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H29" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="I29" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="9">
         <v>2018</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="10">
         <v>200</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I30" s="16" t="s">
+      <c r="I30" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="6">
-        <v>53.91</v>
-      </c>
-      <c r="E31" s="6">
+      <c r="D31" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="9">
         <v>2018</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="10">
         <v>400</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I31" s="16" t="s">
+      <c r="I31" s="6" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1748,534 +1892,534 @@
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="7">
-        <v>1.4344907407407405E-3</v>
-      </c>
-      <c r="E32" s="6">
+      <c r="D32" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="9">
         <v>2021</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="10">
         <v>800</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I32" s="16" t="s">
+      <c r="I32" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="33" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="7">
-        <v>2.8611111111111111E-3</v>
-      </c>
-      <c r="E33" s="6">
+      <c r="D33" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="9">
         <v>2021</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="10">
         <v>1500</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I33" s="16" t="s">
+      <c r="I33" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="7">
-        <v>6.4791666666666669E-3</v>
-      </c>
-      <c r="E34" s="6">
+      <c r="D34" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" s="9">
         <v>2018</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="10">
         <v>3000</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I34" s="16" t="s">
+      <c r="I34" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="35" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="7">
-        <v>1.0947569444444444E-2</v>
-      </c>
-      <c r="E35" s="6">
+      <c r="D35" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="9">
         <v>2022</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="10">
         <v>5000</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I35" s="16" t="s">
+      <c r="I35" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="36" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="7">
-        <v>2.2515509259259259E-2</v>
-      </c>
-      <c r="E36" s="6">
+      <c r="D36" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" s="9">
         <v>2022</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="10">
         <v>10000</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I36" s="16" t="s">
+      <c r="I36" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="7">
-        <v>3.2025462962962958E-3</v>
-      </c>
-      <c r="E37" s="6">
+      <c r="D37" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="9">
         <v>2020</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H37" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I37" s="16" t="s">
+      <c r="I37" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="9">
         <v>2017</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="H38" s="16" t="s">
+      <c r="H38" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I38" s="16" t="s">
+      <c r="I38" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="39" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="6">
-        <v>59.7</v>
-      </c>
-      <c r="E39" s="6">
+      <c r="D39" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E39" s="9">
         <v>1980</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="H39" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I39" s="16" t="s">
+      <c r="I39" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="40" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="7">
-        <v>3.7835648148148147E-3</v>
-      </c>
-      <c r="E40" s="6">
+      <c r="D40" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="9">
         <v>2014</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H40" s="16" t="s">
+      <c r="H40" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I40" s="16" t="s">
+      <c r="I40" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="41" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="7">
-        <v>5.5381944444444437E-3</v>
-      </c>
-      <c r="E41" s="6">
+      <c r="D41" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" s="9">
         <v>2017</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I41" s="16" t="s">
+      <c r="I41" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="42" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="6">
-        <v>1.72</v>
-      </c>
-      <c r="E42" s="6">
+      <c r="D42" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="9">
         <v>1981</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I42" s="16" t="s">
+      <c r="I42" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="43" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="6">
-        <v>5.75</v>
-      </c>
-      <c r="E43" s="6">
+      <c r="D43" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="9">
         <v>2016</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H43" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I43" s="16" t="s">
+      <c r="I43" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="44" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="6">
-        <v>12.55</v>
-      </c>
-      <c r="E44" s="6">
+      <c r="D44" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" s="9">
         <v>2018</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F44" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H44" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I44" s="16" t="s">
+      <c r="I44" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="45" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E45" s="6">
+      <c r="D45" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" s="9">
         <v>2001</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I45" s="16" t="s">
+      <c r="I45" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="46" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="6">
-        <v>13.99</v>
-      </c>
-      <c r="E46" s="6">
+      <c r="D46" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="9">
         <v>2001</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H46" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I46" s="16" t="s">
+      <c r="I46" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="47" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="6">
-        <v>37.159999999999997</v>
-      </c>
-      <c r="E47" s="6">
+      <c r="D47" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E47" s="9">
         <v>2018</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H47" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I47" s="16" t="s">
+      <c r="I47" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="48" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="13">
-        <v>44.3</v>
+      <c r="D48" s="13" t="s">
+        <v>168</v>
       </c>
       <c r="E48" s="13">
         <v>1980</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H48" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I48" s="16" t="s">
+      <c r="I48" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="5">
-        <v>39.47</v>
-      </c>
-      <c r="E49" s="5">
+      <c r="D49" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" s="8">
         <v>2017</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F49" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H49" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I49" s="16" t="s">
+      <c r="I49" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="6">
-        <v>44.48</v>
-      </c>
-      <c r="E50" s="6">
+      <c r="D50" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" s="9">
         <v>2014</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F50" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H50" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I50" s="16" t="s">
+      <c r="I50" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="6">
-        <v>3051</v>
-      </c>
-      <c r="E51" s="6">
+      <c r="D51" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E51" s="9">
         <v>2014</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F51" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H51" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I51" s="16" t="s">
+      <c r="I51" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D52" s="6">
-        <v>49.61</v>
-      </c>
-      <c r="E52" s="6">
+      <c r="D52" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="9">
         <v>2016</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F52" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="H52" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I52" s="16" t="s">
+      <c r="I52" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="7">
-        <v>2.7673611111111111E-3</v>
-      </c>
-      <c r="E53" s="6">
+      <c r="D53" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E53" s="9">
         <v>1992</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F53" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="H53" s="16" t="s">
+      <c r="H53" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I53" s="16" t="s">
+      <c r="I53" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="18" t="s">
         <v>124</v>
       </c>
       <c r="D54" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="E54" s="18" t="s">
+      <c r="E54" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F54" s="20" t="s">
+      <c r="F54" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H54" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="I54" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="J54" s="21" t="s">
+      <c r="H54" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J54" s="7" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working pretty well for overall club records now
</commit_message>
<xml_diff>
--- a/prev_known_and_20022_club_records.xlsx
+++ b/prev_known_and_20022_club_records.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC946F56-938A-4913-BB86-A69DA59047D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0204B908-6BCD-4EF8-B5BC-FB3AEBF653B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="sp7.26k_m_all" localSheetId="0">Sheet1!$G$20</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="176">
   <si>
     <r>
       <t>C&amp;C AC Track and Field records  - Overall club records</t>
@@ -403,9 +406,6 @@
     <t>PV</t>
   </si>
   <si>
-    <t>SP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bogas Kawalko </t>
   </si>
   <si>
@@ -415,9 +415,6 @@
     <t>Dec</t>
   </si>
   <si>
-    <t>100H</t>
-  </si>
-  <si>
     <t>1500SC</t>
   </si>
   <si>
@@ -457,9 +454,6 @@
     <t>HT7.26K</t>
   </si>
   <si>
-    <t>Pen</t>
-  </si>
-  <si>
     <t>4x100</t>
   </si>
   <si>
@@ -638,6 +632,18 @@
   </si>
   <si>
     <t>Use text format when pasting numbers from club records sheet!</t>
+  </si>
+  <si>
+    <t>SP4K</t>
+  </si>
+  <si>
+    <t>100HW</t>
+  </si>
+  <si>
+    <t>PenM35</t>
+  </si>
+  <si>
+    <t>SP7.26K</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0672E4C-1F81-4344-8F80-ED5988EB27BD}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1180,10 +1186,10 @@
         <v>86</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1197,7 +1203,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E2" s="9">
         <v>2022</v>
@@ -1209,10 +1215,10 @@
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1220,7 +1226,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E3" s="9">
         <v>1990</v>
@@ -1232,21 +1238,21 @@
         <v>200</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E4" s="9">
         <v>1989</v>
@@ -1258,10 +1264,10 @@
         <v>400</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1269,7 +1275,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E5" s="9">
         <v>2022</v>
@@ -1281,10 +1287,10 @@
         <v>800</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1292,7 +1298,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E6" s="9">
         <v>2020</v>
@@ -1304,10 +1310,10 @@
         <v>1500</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1315,7 +1321,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E7" s="9">
         <v>2021</v>
@@ -1327,10 +1333,10 @@
         <v>3000</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1338,7 +1344,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E8" s="9">
         <v>2021</v>
@@ -1350,10 +1356,10 @@
         <v>5000</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1361,7 +1367,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E9" s="9">
         <v>2021</v>
@@ -1373,10 +1379,10 @@
         <v>10000</v>
       </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1384,7 +1390,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E10" s="9">
         <v>2021</v>
@@ -1396,10 +1402,10 @@
         <v>87</v>
       </c>
       <c r="H10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1407,22 +1413,22 @@
         <v>21</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E11" s="9">
         <v>1984</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>88</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1430,22 +1436,22 @@
         <v>21</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E12" s="9">
         <v>2012</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>88</v>
       </c>
       <c r="H12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1453,7 +1459,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E13" s="9">
         <v>2022</v>
@@ -1465,10 +1471,10 @@
         <v>89</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1476,7 +1482,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E14" s="9">
         <v>1969</v>
@@ -1488,10 +1494,10 @@
         <v>90</v>
       </c>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1499,7 +1505,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E15" s="9">
         <v>1977</v>
@@ -1511,10 +1517,10 @@
         <v>91</v>
       </c>
       <c r="H15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1522,7 +1528,7 @@
         <v>28</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E16" s="9">
         <v>1977</v>
@@ -1534,10 +1540,10 @@
         <v>92</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1545,7 +1551,7 @@
         <v>30</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E17" s="9">
         <v>1968</v>
@@ -1557,10 +1563,10 @@
         <v>93</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1568,7 +1574,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E18" s="9">
         <v>1978</v>
@@ -1580,10 +1586,10 @@
         <v>94</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1591,7 +1597,7 @@
         <v>34</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E19" s="9">
         <v>1982</v>
@@ -1603,10 +1609,10 @@
         <v>95</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1614,7 +1620,7 @@
         <v>36</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E20" s="9">
         <v>1969</v>
@@ -1623,13 +1629,13 @@
         <v>37</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>96</v>
+        <v>175</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1637,7 +1643,7 @@
         <v>38</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E21" s="9">
         <v>2022</v>
@@ -1646,13 +1652,13 @@
         <v>39</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -1660,22 +1666,22 @@
         <v>40</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E22" s="13">
         <v>1971</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1683,22 +1689,22 @@
         <v>41</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E23" s="8">
         <v>1990</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1706,7 +1712,7 @@
         <v>42</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E24" s="9">
         <v>1970</v>
@@ -1715,13 +1721,13 @@
         <v>37</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1729,7 +1735,7 @@
         <v>43</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E25" s="9">
         <v>2008</v>
@@ -1738,13 +1744,13 @@
         <v>44</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="H25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1752,7 +1758,7 @@
         <v>45</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E26" s="9">
         <v>2022</v>
@@ -1761,13 +1767,13 @@
         <v>46</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1775,7 +1781,7 @@
         <v>47</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>48</v>
@@ -1784,13 +1790,13 @@
         <v>49</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1798,7 +1804,7 @@
         <v>50</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>48</v>
@@ -1807,13 +1813,13 @@
         <v>51</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1836,10 +1842,10 @@
         <v>100</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1859,10 +1865,10 @@
         <v>200</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1870,7 +1876,7 @@
         <v>11</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E31" s="9">
         <v>2018</v>
@@ -1882,10 +1888,10 @@
         <v>400</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1896,7 +1902,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E32" s="9">
         <v>2021</v>
@@ -1908,10 +1914,10 @@
         <v>800</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1919,7 +1925,7 @@
         <v>15</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E33" s="9">
         <v>2021</v>
@@ -1931,10 +1937,10 @@
         <v>1500</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1942,7 +1948,7 @@
         <v>17</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E34" s="9">
         <v>2018</v>
@@ -1954,10 +1960,10 @@
         <v>3000</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1965,7 +1971,7 @@
         <v>18</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E35" s="9">
         <v>2022</v>
@@ -1977,10 +1983,10 @@
         <v>5000</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1988,7 +1994,7 @@
         <v>19</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E36" s="9">
         <v>2022</v>
@@ -2000,10 +2006,10 @@
         <v>10000</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2011,7 +2017,7 @@
         <v>20</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E37" s="9">
         <v>2020</v>
@@ -2023,10 +2029,10 @@
         <v>87</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2043,13 +2049,13 @@
         <v>61</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2057,7 +2063,7 @@
         <v>62</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E39" s="9">
         <v>1980</v>
@@ -2069,10 +2075,10 @@
         <v>89</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2080,7 +2086,7 @@
         <v>64</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E40" s="9">
         <v>2014</v>
@@ -2089,13 +2095,13 @@
         <v>65</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2103,7 +2109,7 @@
         <v>24</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E41" s="9">
         <v>2017</v>
@@ -2115,10 +2121,10 @@
         <v>90</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2126,7 +2132,7 @@
         <v>67</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E42" s="9">
         <v>1981</v>
@@ -2138,10 +2144,10 @@
         <v>92</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2149,7 +2155,7 @@
         <v>69</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E43" s="9">
         <v>2016</v>
@@ -2161,10 +2167,10 @@
         <v>93</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2172,7 +2178,7 @@
         <v>71</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E44" s="9">
         <v>2018</v>
@@ -2184,10 +2190,10 @@
         <v>94</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2195,7 +2201,7 @@
         <v>73</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E45" s="9">
         <v>2001</v>
@@ -2207,10 +2213,10 @@
         <v>95</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2218,7 +2224,7 @@
         <v>36</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E46" s="9">
         <v>2001</v>
@@ -2227,13 +2233,13 @@
         <v>75</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2241,7 +2247,7 @@
         <v>38</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E47" s="9">
         <v>2018</v>
@@ -2250,13 +2256,13 @@
         <v>76</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="3:9" ht="15" x14ac:dyDescent="0.2">
@@ -2264,7 +2270,7 @@
         <v>77</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E48" s="13">
         <v>1980</v>
@@ -2273,13 +2279,13 @@
         <v>79</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2287,7 +2293,7 @@
         <v>78</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E49" s="8">
         <v>2017</v>
@@ -2296,13 +2302,13 @@
         <v>80</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2310,7 +2316,7 @@
         <v>81</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E50" s="9">
         <v>2014</v>
@@ -2319,13 +2325,13 @@
         <v>82</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2333,7 +2339,7 @@
         <v>43</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E51" s="9">
         <v>2014</v>
@@ -2342,13 +2348,13 @@
         <v>83</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2356,7 +2362,7 @@
         <v>47</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E52" s="9">
         <v>2016</v>
@@ -2365,13 +2371,13 @@
         <v>84</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2379,7 +2385,7 @@
         <v>50</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E53" s="9">
         <v>1992</v>
@@ -2388,39 +2394,39 @@
         <v>85</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="C54" s="18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.2">

</xml_diff>